<commit_message>
add sales20 and balances to accounting
</commit_message>
<xml_diff>
--- a/templates/InvoicablePayables.xlsx
+++ b/templates/InvoicablePayables.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1827DA-52CA-445A-AB51-741D89D0382B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03DEE3A-BD6E-4A51-89CA-52CFD1AD0F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31275" yWindow="-4875" windowWidth="24105" windowHeight="15600" activeTab="2" xr2:uid="{932300A4-E802-4396-9D5F-5FC3E73FEA3E}"/>
+    <workbookView xWindow="35880" yWindow="-2910" windowWidth="24105" windowHeight="15600" activeTab="3" xr2:uid="{932300A4-E802-4396-9D5F-5FC3E73FEA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="MRI PAYABLES" sheetId="1" r:id="rId1"/>
     <sheet name="MRI Invoicable" sheetId="2" r:id="rId2"/>
     <sheet name="Sales" sheetId="3" r:id="rId3"/>
+    <sheet name="BALANCE MRI" sheetId="4" r:id="rId4"/>
+    <sheet name="BALANCE CTL" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t xml:space="preserve"> METCUT RECHERCHES S.A.S</t>
   </si>
@@ -168,13 +170,34 @@
   </si>
   <si>
     <t xml:space="preserve"> $ / €UROS</t>
+  </si>
+  <si>
+    <t>BALANCE</t>
+  </si>
+  <si>
+    <t>N°Inv Mri/Mrsa</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>N° JOB MRSA</t>
+  </si>
+  <si>
+    <t>N° JOB MRI</t>
+  </si>
+  <si>
+    <t>AMOUNT $</t>
+  </si>
+  <si>
+    <t>AMOUNT €</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="14">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-40C]d\ mmmm\ yyyy;@"/>
@@ -183,11 +206,14 @@
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00\ [$€-40C]"/>
-    <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="172" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="175" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +293,13 @@
       <b/>
       <u/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,7 +405,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,68 +510,68 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -548,6 +581,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1085,9 +1150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1F078A-7D2E-4850-8207-A065F68FE74A}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,9 +1209,7 @@
       <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
-        <v>2020</v>
-      </c>
+      <c r="A3" s="34"/>
       <c r="B3" s="35"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -1285,4 +1348,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DBC17F-D4B8-4857-A478-DCAEDCBA9AE0}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="71" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="73" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717CAF6A-A3D7-4E49-A906-38F920604C2D}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="14.7109375" style="11" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" style="70" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix accounting juillet 2020
</commit_message>
<xml_diff>
--- a/templates/InvoicablePayables.xlsx
+++ b/templates/InvoicablePayables.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03DEE3A-BD6E-4A51-89CA-52CFD1AD0F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E35388-11FB-4DC1-BA91-63619F68C707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35880" yWindow="-2910" windowWidth="24105" windowHeight="15600" activeTab="3" xr2:uid="{932300A4-E802-4396-9D5F-5FC3E73FEA3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{932300A4-E802-4396-9D5F-5FC3E73FEA3E}"/>
   </bookViews>
   <sheets>
-    <sheet name="MRI PAYABLES" sheetId="1" r:id="rId1"/>
-    <sheet name="MRI Invoicable" sheetId="2" r:id="rId2"/>
+    <sheet name="MRSAS PAYABLES" sheetId="1" r:id="rId1"/>
+    <sheet name="MRSAS Invoicable" sheetId="2" r:id="rId2"/>
     <sheet name="Sales" sheetId="3" r:id="rId3"/>
     <sheet name="BALANCE MRI" sheetId="4" r:id="rId4"/>
     <sheet name="BALANCE CTL" sheetId="5" r:id="rId5"/>
@@ -197,7 +197,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="14">
+  <numFmts count="12">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-40C]d\ mmmm\ yyyy;@"/>
@@ -209,8 +209,6 @@
     <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="171" formatCode="#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="172" formatCode="[$$-409]#,##0.00"/>
-    <numFmt numFmtId="173" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="175" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
@@ -405,7 +403,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,17 +592,8 @@
     <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -612,6 +601,12 @@
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -941,15 +936,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3C9DF5-2C19-4954-B528-796229C8BF3C}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" style="14" customWidth="1"/>
-    <col min="2" max="8" width="15.28515625" style="11" customWidth="1"/>
+    <col min="2" max="7" width="15.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="11" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1019,7 +1015,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1354,15 +1350,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DBC17F-D4B8-4857-A478-DCAEDCBA9AE0}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="71" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="73" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="68" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="70" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1392,13 +1388,13 @@
       <c r="D5" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="67" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1413,13 +1409,14 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="14.7109375" style="11" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" style="70" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="60" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="49" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1449,13 +1446,13 @@
       <c r="D5" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="67" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>